<commit_message>
more fixes to differential output board
</commit_message>
<xml_diff>
--- a/bom/differential_output_board.xlsx
+++ b/bom/differential_output_board.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Electronics/EAGLE/lichtenstein_onion/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7EA6A3-056F-5A4B-95C1-4ABBD265440F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74B2B7-3D1F-BF49-8ED7-D502F06EA98F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9200" yWindow="980" windowWidth="32740" windowHeight="23800" xr2:uid="{46863911-3D57-E942-A477-216F516C7958}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -916,7 +916,7 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1180,26 +1180,26 @@
       <c r="F12" s="13"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" ht="17">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="17">
+      <c r="A13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="17"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:7" s="14" customFormat="1" ht="17">
       <c r="A14" s="12" t="s">
@@ -1537,26 +1537,26 @@
       </c>
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:7" ht="17">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:7" s="14" customFormat="1" ht="17">
+      <c r="A30" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:7" ht="17">
       <c r="A31" s="10" t="s">

</xml_diff>